<commit_message>
Added version 2_1 for automatic batch processing.
</commit_message>
<xml_diff>
--- a/RECC_ModelConfig_List.xlsx
+++ b/RECC_ModelConfig_List.xlsx
@@ -8,15 +8,16 @@
   </bookViews>
   <sheets>
     <sheet name="RECC_Config_IRP_V1" sheetId="1" r:id="rId1"/>
-    <sheet name="SingleTestRun" sheetId="2" r:id="rId2"/>
-    <sheet name="GroupTestRun" sheetId="3" r:id="rId3"/>
+    <sheet name="Evaluate_Config_IRP_V1" sheetId="4" r:id="rId2"/>
+    <sheet name="SingleTestRun" sheetId="2" r:id="rId3"/>
+    <sheet name="GroupTestRun" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1828" uniqueCount="196">
   <si>
     <t>Sheet_Name</t>
   </si>
@@ -165,34 +166,451 @@
     <t>G7_RES_Sensitivity</t>
   </si>
   <si>
-    <t>UK_2019_6_14__22_12_47</t>
-  </si>
-  <si>
-    <t>UK_2019_6_14__22_14_23_FYI_EoL_RUS_LTE</t>
-  </si>
-  <si>
-    <t>UK_2019_6_14__22_15_44_FYI_EoL_MSU_DOS_RUS_LTE</t>
-  </si>
-  <si>
-    <t>UK_2019_6_14__22_17_3_FYI_EoL_MSU_DOS_RUS_LTE_MIU</t>
-  </si>
-  <si>
-    <t>UK_2019_6_14__22_18_23_FYI_EoL_MSU_DOS_RUS_LTE_MIU</t>
-  </si>
-  <si>
-    <t>Folder names (created by ODYM-RECC)</t>
-  </si>
-  <si>
     <t>Include_REStrategy_UsingLessMaterialByDesign</t>
   </si>
   <si>
     <t>ULD</t>
+  </si>
+  <si>
+    <t>G7Test</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>G7</t>
+  </si>
+  <si>
+    <t>EU28</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Cascade</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>Regional scope</t>
+  </si>
+  <si>
+    <t>Type (cascade vs. scenario)</t>
+  </si>
+  <si>
+    <t>ENDOFLIST</t>
+  </si>
+  <si>
+    <t>Germany_2019_6_17__22_51_14_PassVehs</t>
+  </si>
+  <si>
+    <t>Germany_2019_6_17__22_51_52_PassVehs_FYI_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Germany_2019_6_17__22_52_32_PassVehs_FYI_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Germany_2019_6_17__22_53_12_PassVehs_FYI_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Germany_2019_6_17__22_53_54_PassVehs_FYI_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>Germany_2019_6_17__22_54_37_ResBlds</t>
+  </si>
+  <si>
+    <t>Germany_2019_6_17__22_55_19_ResBlds_FYI_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Germany_2019_6_17__22_55_59_ResBlds_FYI_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Germany_2019_6_17__22_56_40_ResBlds_FYI_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Germany_2019_6_17__22_57_21_ResBlds_FYI_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>Italy_2019_6_17__22_58_4_PassVehs</t>
+  </si>
+  <si>
+    <t>Italy_2019_6_17__23_0_49_PassVehs_FYI_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Italy_2019_6_17__23_1_32_PassVehs_FYI_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Italy_2019_6_17__23_2_14_PassVehs_FYI_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Italy_2019_6_17__23_2_57_PassVehs_FYI_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>Italy_2019_6_17__23_3_39_ResBlds</t>
+  </si>
+  <si>
+    <t>Italy_2019_6_17__23_4_23_ResBlds_FYI_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Italy_2019_6_17__23_5_7_ResBlds_FYI_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Italy_2019_6_17__23_5_49_ResBlds_FYI_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Italy_2019_6_17__23_6_31_ResBlds_FYI_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>France_2019_6_17__23_7_15_PassVehs</t>
+  </si>
+  <si>
+    <t>France_2019_6_17__23_10_3_PassVehs_FYI_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>France_2019_6_17__23_10_47_PassVehs_FYI_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>France_2019_6_17__23_11_30_PassVehs_FYI_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>France_2019_6_17__23_12_11_PassVehs_FYI_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>France_2019_6_17__23_12_53_ResBlds</t>
+  </si>
+  <si>
+    <t>France_2019_6_17__23_13_36_ResBlds_FYI_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>France_2019_6_17__23_14_19_ResBlds_FYI_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>France_2019_6_17__23_15_2_ResBlds_FYI_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>France_2019_6_17__23_15_45_ResBlds_FYI_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>UK_2019_6_17__23_16_29_PassVehs</t>
+  </si>
+  <si>
+    <t>UK_2019_6_17__23_17_12_PassVehs_FYI_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>UK_2019_6_17__23_17_56_PassVehs_FYI_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>UK_2019_6_17__23_18_39_PassVehs_FYI_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>UK_2019_6_17__23_19_22_PassVehs_FYI_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>UK_2019_6_17__23_20_5_ResBlds</t>
+  </si>
+  <si>
+    <t>UK_2019_6_17__23_20_46_ResBlds_FYI_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>UK_2019_6_17__23_21_30_ResBlds_FYI_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>UK_2019_6_17__23_22_13_ResBlds_FYI_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>UK_2019_6_17__23_22_56_ResBlds_FYI_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>Japan_2019_6_17__23_23_37_PassVehs</t>
+  </si>
+  <si>
+    <t>Japan_2019_6_17__23_26_23_PassVehs_FYI_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Japan_2019_6_17__23_27_7_PassVehs_FYI_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Japan_2019_6_17__23_27_49_PassVehs_FYI_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Japan_2019_6_17__23_28_31_PassVehs_FYI_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>Japan_2019_6_17__23_29_12_ResBlds</t>
+  </si>
+  <si>
+    <t>Japan_2019_6_17__23_29_55_ResBlds_FYI_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Japan_2019_6_17__23_30_38_ResBlds_FYI_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Japan_2019_6_17__23_31_21_ResBlds_FYI_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Japan_2019_6_17__23_32_3_ResBlds_FYI_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>Canada_2019_6_17__23_32_46_PassVehs</t>
+  </si>
+  <si>
+    <t>Canada_2019_6_17__23_35_32_PassVehs_FYI_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Canada_2019_6_17__23_36_16_PassVehs_FYI_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Canada_2019_6_17__23_36_59_PassVehs_FYI_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Canada_2019_6_17__23_37_41_PassVehs_FYI_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>Canada_2019_6_17__23_38_24_ResBlds</t>
+  </si>
+  <si>
+    <t>Canada_2019_6_17__23_39_7_ResBlds_FYI_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Canada_2019_6_17__23_39_50_ResBlds_FYI_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Canada_2019_6_17__23_40_33_ResBlds_FYI_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>Canada_2019_6_17__23_41_17_ResBlds_FYI_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>USA_2019_6_17__23_41_59_PassVehs</t>
+  </si>
+  <si>
+    <t>USA_2019_6_17__23_42_43_PassVehs_FYI_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>USA_2019_6_17__23_43_27_PassVehs_FYI_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>USA_2019_6_17__23_44_11_PassVehs_FYI_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>USA_2019_6_17__23_44_54_PassVehs_FYI_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>USA_2019_6_17__23_45_38_ResBlds</t>
+  </si>
+  <si>
+    <t>USA_2019_6_17__23_46_21_ResBlds_FYI_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>USA_2019_6_17__23_47_4_ResBlds_FYI_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>USA_2019_6_17__23_47_48_ResBlds_FYI_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>USA_2019_6_17__23_48_32_ResBlds_FYI_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>G7_2019_6_17__23_49_17_PassVehs</t>
+  </si>
+  <si>
+    <t>G7_2019_6_17__23_51_41_PassVehs_FYI_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>G7_2019_6_17__23_54_4_PassVehs_FYI_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>G7_2019_6_17__23_56_26_PassVehs_FYI_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>G7_2019_6_17__23_58_48_PassVehs_FYI_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>G7_2019_6_18__0_1_10_ResBlds</t>
+  </si>
+  <si>
+    <t>G7_2019_6_18__0_3_31_ResBlds_FYI_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>G7_2019_6_18__0_5_53_ResBlds_FYI_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>G7_2019_6_18__0_8_14_ResBlds_FYI_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>G7_2019_6_18__6_15_24_ResBlds_FYI_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>EU28_2019_6_18__6_17_34_PassVehs</t>
+  </si>
+  <si>
+    <t>EU28_2019_6_18__6_22_39_PassVehs_FYI_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>EU28_2019_6_18__6_25_28_PassVehs_FYI_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>EU28_2019_6_18__6_28_19_PassVehs_FYI_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>EU28_2019_6_18__6_31_9_PassVehs_FYI_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>EU28_2019_6_18__6_34_0_ResBlds</t>
+  </si>
+  <si>
+    <t>EU28_2019_6_18__6_36_52_ResBlds_FYI_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>EU28_2019_6_18__6_39_43_ResBlds_FYI_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>EU28_2019_6_18__6_42_37_ResBlds_FYI_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>EU28_2019_6_18__6_45_31_ResBlds_FYI_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>India_2019_6_18__6_48_27_PassVehs</t>
+  </si>
+  <si>
+    <t>India_2019_6_18__6_49_13_PassVehs_FYI_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>India_2019_6_18__6_49_57_PassVehs_FYI_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>India_2019_6_18__6_50_39_PassVehs_FYI_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>India_2019_6_18__6_51_24_PassVehs_FYI_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>India_2019_6_18__6_52_9_ResBlds</t>
+  </si>
+  <si>
+    <t>India_2019_6_18__6_52_52_ResBlds_FYI_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>India_2019_6_18__6_53_35_ResBlds_FYI_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>India_2019_6_18__6_54_18_ResBlds_FYI_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>India_2019_6_18__6_55_2_ResBlds_FYI_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>China_2019_6_18__6_55_46_PassVehs</t>
+  </si>
+  <si>
+    <t>China_2019_6_18__6_58_31_PassVehs_FYI_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>China_2019_6_18__6_59_16_PassVehs_FYI_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>China_2019_6_18__7_0_1_PassVehs_FYI_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>China_2019_6_18__7_0_49_PassVehs_FYI_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>China_2019_6_18__7_1_34_ResBlds</t>
+  </si>
+  <si>
+    <t>China_2019_6_18__7_2_18_ResBlds_FYI_EoL_RUS_LTE</t>
+  </si>
+  <si>
+    <t>China_2019_6_18__7_3_2_ResBlds_FYI_EoL_MSU_RUS_LTE</t>
+  </si>
+  <si>
+    <t>China_2019_6_18__7_3_47_ResBlds_FYI_EoL_MSU_ULD_RUS_LTE</t>
+  </si>
+  <si>
+    <t>China_2019_6_18__7_4_30_ResBlds_FYI_EoL_MSU_ULD_RUS_LTE_MIU</t>
+  </si>
+  <si>
+    <t>G7_2019_6_18__7_5_15_PassVehs_FYI</t>
+  </si>
+  <si>
+    <t>G7_2019_6_18__7_7_35_PassVehs_EoL</t>
+  </si>
+  <si>
+    <t>G7_2019_6_18__7_9_59_PassVehs_MSU</t>
+  </si>
+  <si>
+    <t>G7_2019_6_18__7_12_21_PassVehs_ULD</t>
+  </si>
+  <si>
+    <t>G7_2019_6_18__7_14_44_PassVehs_RUS</t>
+  </si>
+  <si>
+    <t>G7_2019_6_18__7_17_8_PassVehs_LTE</t>
+  </si>
+  <si>
+    <t>G7_2019_6_18__7_19_31_PassVehs_MIU</t>
+  </si>
+  <si>
+    <t>G7_2019_6_18__7_21_53_PassVehs</t>
+  </si>
+  <si>
+    <t>G7_2019_6_18__7_24_14_ResBlds_FYI</t>
+  </si>
+  <si>
+    <t>G7_2019_6_18__7_26_37_ResBlds_EoL</t>
+  </si>
+  <si>
+    <t>G7_2019_6_18__7_29_0_ResBlds_MSU</t>
+  </si>
+  <si>
+    <t>G7_2019_6_18__7_31_24_ResBlds_ULD</t>
+  </si>
+  <si>
+    <t>G7_2019_6_18__7_33_49_ResBlds_RUS</t>
+  </si>
+  <si>
+    <t>G7_2019_6_18__7_36_13_ResBlds_LTE</t>
+  </si>
+  <si>
+    <t>G7_2019_6_18__7_38_37_ResBlds_MIU</t>
+  </si>
+  <si>
+    <t>G7_2019_6_18__7_41_0_ResBlds</t>
+  </si>
+  <si>
+    <t>Folder names (copy past from Python list 'ResultFolders')</t>
+  </si>
+  <si>
+    <t>!!! No-RES reference case was inserted here from previous model run for G7 above!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -251,7 +669,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -540,23 +958,23 @@
   <dimension ref="A2:N129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="C106" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="53.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1"/>
-    <col min="6" max="6" width="9.77734375" customWidth="1"/>
+    <col min="1" max="1" width="5.68359375" customWidth="1"/>
+    <col min="2" max="2" width="23.3125" customWidth="1"/>
+    <col min="3" max="3" width="17.41796875" customWidth="1"/>
+    <col min="4" max="4" width="18.1015625" customWidth="1"/>
+    <col min="5" max="5" width="11.1015625" customWidth="1"/>
+    <col min="6" max="6" width="9.7890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="D2" t="s">
         <v>16</v>
       </c>
@@ -570,7 +988,7 @@
         <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -591,10 +1009,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>54</v>
-      </c>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -614,7 +1030,7 @@
         <v>6</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>7</v>
@@ -635,7 +1051,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
         <v>26</v>
       </c>
@@ -676,7 +1092,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" t="s">
         <v>2</v>
       </c>
@@ -714,7 +1130,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" t="s">
         <v>2</v>
       </c>
@@ -752,7 +1168,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" t="s">
         <v>2</v>
       </c>
@@ -790,7 +1206,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" t="s">
         <v>2</v>
       </c>
@@ -828,7 +1244,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" t="s">
         <v>2</v>
       </c>
@@ -866,7 +1282,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C10" t="s">
         <v>2</v>
       </c>
@@ -904,7 +1320,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C11" t="s">
         <v>2</v>
       </c>
@@ -942,7 +1358,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C12" t="s">
         <v>2</v>
       </c>
@@ -980,7 +1396,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C13" t="s">
         <v>2</v>
       </c>
@@ -1018,7 +1434,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" t="s">
         <v>28</v>
       </c>
@@ -1059,7 +1475,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C15" t="s">
         <v>29</v>
       </c>
@@ -1097,7 +1513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C16" t="s">
         <v>29</v>
       </c>
@@ -1135,7 +1551,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C17" t="s">
         <v>29</v>
       </c>
@@ -1173,7 +1589,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C18" t="s">
         <v>29</v>
       </c>
@@ -1211,7 +1627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C19" t="s">
         <v>29</v>
       </c>
@@ -1249,7 +1665,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C20" t="s">
         <v>29</v>
       </c>
@@ -1287,7 +1703,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C21" t="s">
         <v>29</v>
       </c>
@@ -1325,7 +1741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C22" t="s">
         <v>29</v>
       </c>
@@ -1363,7 +1779,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C23" t="s">
         <v>29</v>
       </c>
@@ -1401,7 +1817,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" t="s">
         <v>30</v>
       </c>
@@ -1442,7 +1858,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C25" t="s">
         <v>31</v>
       </c>
@@ -1480,7 +1896,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C26" t="s">
         <v>31</v>
       </c>
@@ -1518,7 +1934,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C27" t="s">
         <v>31</v>
       </c>
@@ -1556,7 +1972,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C28" t="s">
         <v>31</v>
       </c>
@@ -1594,7 +2010,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C29" t="s">
         <v>31</v>
       </c>
@@ -1632,7 +2048,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C30" t="s">
         <v>31</v>
       </c>
@@ -1670,7 +2086,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C31" t="s">
         <v>31</v>
       </c>
@@ -1708,7 +2124,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C32" t="s">
         <v>31</v>
       </c>
@@ -1746,7 +2162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C33" t="s">
         <v>31</v>
       </c>
@@ -1784,7 +2200,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" t="s">
         <v>32</v>
       </c>
@@ -1825,7 +2241,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C35" t="s">
         <v>33</v>
       </c>
@@ -1863,7 +2279,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C36" t="s">
         <v>33</v>
       </c>
@@ -1901,7 +2317,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C37" t="s">
         <v>33</v>
       </c>
@@ -1939,7 +2355,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C38" t="s">
         <v>33</v>
       </c>
@@ -1977,7 +2393,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C39" t="s">
         <v>33</v>
       </c>
@@ -2015,7 +2431,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C40" t="s">
         <v>33</v>
       </c>
@@ -2053,7 +2469,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C41" t="s">
         <v>33</v>
       </c>
@@ -2091,7 +2507,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C42" t="s">
         <v>33</v>
       </c>
@@ -2129,7 +2545,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C43" t="s">
         <v>33</v>
       </c>
@@ -2167,7 +2583,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B44" t="s">
         <v>34</v>
       </c>
@@ -2208,7 +2624,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C45" t="s">
         <v>35</v>
       </c>
@@ -2246,7 +2662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C46" t="s">
         <v>35</v>
       </c>
@@ -2284,7 +2700,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C47" t="s">
         <v>35</v>
       </c>
@@ -2322,7 +2738,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C48" t="s">
         <v>35</v>
       </c>
@@ -2360,7 +2776,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C49" t="s">
         <v>35</v>
       </c>
@@ -2398,7 +2814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C50" t="s">
         <v>35</v>
       </c>
@@ -2436,7 +2852,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C51" t="s">
         <v>35</v>
       </c>
@@ -2474,7 +2890,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C52" t="s">
         <v>35</v>
       </c>
@@ -2512,7 +2928,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C53" t="s">
         <v>35</v>
       </c>
@@ -2550,7 +2966,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B54" t="s">
         <v>36</v>
       </c>
@@ -2591,7 +3007,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C55" t="s">
         <v>37</v>
       </c>
@@ -2629,7 +3045,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C56" t="s">
         <v>37</v>
       </c>
@@ -2667,7 +3083,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C57" t="s">
         <v>37</v>
       </c>
@@ -2705,7 +3121,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C58" t="s">
         <v>37</v>
       </c>
@@ -2743,7 +3159,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C59" t="s">
         <v>37</v>
       </c>
@@ -2781,7 +3197,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C60" t="s">
         <v>37</v>
       </c>
@@ -2819,7 +3235,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C61" t="s">
         <v>37</v>
       </c>
@@ -2857,7 +3273,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C62" t="s">
         <v>37</v>
       </c>
@@ -2895,7 +3311,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C63" t="s">
         <v>37</v>
       </c>
@@ -2933,7 +3349,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B64" t="s">
         <v>38</v>
       </c>
@@ -2974,7 +3390,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C65" t="s">
         <v>39</v>
       </c>
@@ -3012,7 +3428,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C66" t="s">
         <v>39</v>
       </c>
@@ -3050,7 +3466,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C67" t="s">
         <v>39</v>
       </c>
@@ -3088,7 +3504,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C68" t="s">
         <v>39</v>
       </c>
@@ -3126,7 +3542,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C69" t="s">
         <v>39</v>
       </c>
@@ -3164,7 +3580,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C70" t="s">
         <v>39</v>
       </c>
@@ -3202,7 +3618,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C71" t="s">
         <v>39</v>
       </c>
@@ -3240,7 +3656,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C72" t="s">
         <v>39</v>
       </c>
@@ -3278,7 +3694,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C73" t="s">
         <v>39</v>
       </c>
@@ -3316,7 +3732,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B74" t="s">
         <v>40</v>
       </c>
@@ -3357,7 +3773,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C75" t="s">
         <v>41</v>
       </c>
@@ -3395,7 +3811,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C76" t="s">
         <v>41</v>
       </c>
@@ -3433,7 +3849,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C77" t="s">
         <v>41</v>
       </c>
@@ -3471,7 +3887,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C78" t="s">
         <v>41</v>
       </c>
@@ -3509,7 +3925,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C79" t="s">
         <v>41</v>
       </c>
@@ -3547,7 +3963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C80" t="s">
         <v>41</v>
       </c>
@@ -3585,7 +4001,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C81" t="s">
         <v>41</v>
       </c>
@@ -3623,7 +4039,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C82" t="s">
         <v>41</v>
       </c>
@@ -3661,7 +4077,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C83" t="s">
         <v>41</v>
       </c>
@@ -3699,7 +4115,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B84" t="s">
         <v>42</v>
       </c>
@@ -3740,7 +4156,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C85" t="s">
         <v>43</v>
       </c>
@@ -3778,7 +4194,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C86" t="s">
         <v>43</v>
       </c>
@@ -3816,7 +4232,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C87" t="s">
         <v>43</v>
       </c>
@@ -3854,7 +4270,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C88" t="s">
         <v>43</v>
       </c>
@@ -3892,7 +4308,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C89" t="s">
         <v>43</v>
       </c>
@@ -3930,7 +4346,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C90" t="s">
         <v>43</v>
       </c>
@@ -3968,7 +4384,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C91" t="s">
         <v>43</v>
       </c>
@@ -4006,7 +4422,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C92" t="s">
         <v>43</v>
       </c>
@@ -4044,7 +4460,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C93" t="s">
         <v>43</v>
       </c>
@@ -4082,7 +4498,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B94" t="s">
         <v>44</v>
       </c>
@@ -4123,7 +4539,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C95" t="s">
         <v>45</v>
       </c>
@@ -4161,7 +4577,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C96" t="s">
         <v>45</v>
       </c>
@@ -4199,7 +4615,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C97" t="s">
         <v>45</v>
       </c>
@@ -4237,7 +4653,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C98" t="s">
         <v>45</v>
       </c>
@@ -4275,7 +4691,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C99" t="s">
         <v>45</v>
       </c>
@@ -4313,7 +4729,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C100" t="s">
         <v>45</v>
       </c>
@@ -4351,7 +4767,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C101" t="s">
         <v>45</v>
       </c>
@@ -4389,7 +4805,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C102" t="s">
         <v>45</v>
       </c>
@@ -4427,7 +4843,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C103" t="s">
         <v>45</v>
       </c>
@@ -4465,7 +4881,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B104" t="s">
         <v>46</v>
       </c>
@@ -4506,7 +4922,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C105" t="s">
         <v>47</v>
       </c>
@@ -4544,7 +4960,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C106" t="s">
         <v>47</v>
       </c>
@@ -4582,7 +4998,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C107" t="s">
         <v>47</v>
       </c>
@@ -4620,7 +5036,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C108" t="s">
         <v>47</v>
       </c>
@@ -4658,7 +5074,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C109" t="s">
         <v>47</v>
       </c>
@@ -4696,7 +5112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C110" t="s">
         <v>47</v>
       </c>
@@ -4734,7 +5150,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C111" t="s">
         <v>47</v>
       </c>
@@ -4772,7 +5188,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C112" t="s">
         <v>47</v>
       </c>
@@ -4810,7 +5226,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="113" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C113" t="s">
         <v>47</v>
       </c>
@@ -4848,7 +5264,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B114" t="s">
         <v>48</v>
       </c>
@@ -4889,7 +5305,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C115" t="s">
         <v>41</v>
       </c>
@@ -4927,7 +5343,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C116" t="s">
         <v>41</v>
       </c>
@@ -4965,7 +5381,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C117" t="s">
         <v>41</v>
       </c>
@@ -5003,7 +5419,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="118" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C118" t="s">
         <v>41</v>
       </c>
@@ -5041,7 +5457,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C119" t="s">
         <v>41</v>
       </c>
@@ -5079,7 +5495,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C120" t="s">
         <v>41</v>
       </c>
@@ -5117,7 +5533,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="121" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C121" t="s">
         <v>41</v>
       </c>
@@ -5155,7 +5571,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="122" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C122" t="s">
         <v>41</v>
       </c>
@@ -5193,7 +5609,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C123" t="s">
         <v>41</v>
       </c>
@@ -5231,7 +5647,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="124" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C124" t="s">
         <v>41</v>
       </c>
@@ -5269,7 +5685,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="125" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C125" t="s">
         <v>41</v>
       </c>
@@ -5307,7 +5723,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C126" t="s">
         <v>41</v>
       </c>
@@ -5345,7 +5761,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C127" t="s">
         <v>41</v>
       </c>
@@ -5383,7 +5799,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C128" t="s">
         <v>41</v>
       </c>
@@ -5421,7 +5837,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="3:14" x14ac:dyDescent="0.3">
+    <row r="129" spans="3:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C129" t="s">
         <v>41</v>
       </c>
@@ -5466,21 +5882,774 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E130"/>
+  <sheetViews>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="E121" sqref="E121"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="4" max="4" width="64.578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D31" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D33" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D34" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D35" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D36" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D37" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D38" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D39" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D41" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B42" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D43" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D44" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D45" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D46" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D47" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D48" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D49" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D50" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D51" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B52" t="s">
+        <v>57</v>
+      </c>
+      <c r="C52" t="s">
+        <v>63</v>
+      </c>
+      <c r="D52" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D53" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D55" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D56" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D57" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D58" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D59" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D60" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D61" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B62" t="s">
+        <v>58</v>
+      </c>
+      <c r="C62" t="s">
+        <v>63</v>
+      </c>
+      <c r="D62" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D63" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D64" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D65" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D66" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D67" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D68" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D69" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D70" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D71" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B72" t="s">
+        <v>59</v>
+      </c>
+      <c r="C72" t="s">
+        <v>63</v>
+      </c>
+      <c r="D72" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D73" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D74" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D75" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D76" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D77" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D78" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D79" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D80" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D81" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B82" t="s">
+        <v>60</v>
+      </c>
+      <c r="C82" t="s">
+        <v>63</v>
+      </c>
+      <c r="D82" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D83" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D84" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D85" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D86" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D87" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D88" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D89" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D90" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D91" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B92" t="s">
+        <v>61</v>
+      </c>
+      <c r="C92" t="s">
+        <v>63</v>
+      </c>
+      <c r="D92" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D93" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D94" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D95" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D96" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D97" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D98" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D99" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D100" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D101" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B102" t="s">
+        <v>62</v>
+      </c>
+      <c r="C102" t="s">
+        <v>63</v>
+      </c>
+      <c r="D102" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D103" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D104" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D105" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D106" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D107" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D108" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D109" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D110" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D111" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="112" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B112" t="s">
+        <v>59</v>
+      </c>
+      <c r="C112" t="s">
+        <v>64</v>
+      </c>
+      <c r="D112" t="s">
+        <v>138</v>
+      </c>
+      <c r="E112" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="113" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D113" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="114" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D114" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="115" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D115" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="116" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D116" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="117" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D117" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="118" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D118" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="119" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D119" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="120" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D120" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="121" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D121" t="s">
+        <v>143</v>
+      </c>
+      <c r="E121" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="122" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D122" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="123" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D123" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="124" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D124" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="125" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D125" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="126" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D126" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="127" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D127" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="128" spans="4:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D128" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="D129" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B130" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="53.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.21875" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="24.20703125" customWidth="1"/>
+    <col min="3" max="3" width="22.1015625" customWidth="1"/>
+    <col min="4" max="4" width="16.1015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="D2" t="s">
         <v>16</v>
       </c>
@@ -5494,7 +6663,7 @@
         <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -5515,10 +6684,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>54</v>
-      </c>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -5538,7 +6705,7 @@
         <v>6</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>7</v>
@@ -5559,15 +6726,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -5588,7 +6755,7 @@
         <v>15</v>
       </c>
       <c r="K4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L4" t="s">
         <v>14</v>
@@ -5605,20 +6772,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="53.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="D2" t="s">
         <v>16</v>
       </c>
@@ -5632,7 +6799,7 @@
         <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
@@ -5653,10 +6820,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>54</v>
-      </c>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -5676,7 +6841,7 @@
         <v>6</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>7</v>
@@ -5697,10 +6862,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>49</v>
-      </c>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
         <v>32</v>
       </c>
@@ -5741,12 +6903,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
@@ -5782,12 +6941,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>51</v>
-      </c>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
         <v>27</v>
@@ -5823,12 +6979,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
         <v>27</v>
@@ -5864,12 +7017,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>53</v>
-      </c>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>

</xml_diff>